<commit_message>
Add A B testing
</commit_message>
<xml_diff>
--- a/DataAnalytics/Notes_Hands-On-Data-Science-for-Marketing/CLV-algorithm.xlsx
+++ b/DataAnalytics/Notes_Hands-On-Data-Science-for-Marketing/CLV-algorithm.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baha Tegar\Desktop\Preparation\DataAnalytics\Notes_Hands-On-Data-Science-for-Marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F296716-D1C6-48C6-8B24-E5D02F2C3777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97ABCE6-2781-44B8-B18D-71B36711A4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{EE61D2FF-6439-4F37-889D-593EC2676691}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{EE61D2FF-6439-4F37-889D-593EC2676691}"/>
   </bookViews>
   <sheets>
     <sheet name="Traditional-algorithm" sheetId="1" r:id="rId1"/>
     <sheet name="Predictive-algorithm" sheetId="2" r:id="rId2"/>
     <sheet name="Exercise" sheetId="3" r:id="rId3"/>
+    <sheet name="cohort" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="156">
   <si>
     <t>NOTE: Cost capital commonly assume 10-15%</t>
   </si>
@@ -432,6 +433,78 @@
   </si>
   <si>
     <t>NOTE: Average customer lifespan = 1 / churn rate</t>
+  </si>
+  <si>
+    <t>CUSTOMER RETENTION &amp; COHORT ANALYSIS</t>
+  </si>
+  <si>
+    <t>Let there is customer cohort:</t>
+  </si>
+  <si>
+    <t>SrNo.</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Customer Cohort</t>
+  </si>
+  <si>
+    <t>CUSTOMER RETENTION BY COHORT</t>
+  </si>
+  <si>
+    <t>NET REVENUE BY COHORT</t>
+  </si>
+  <si>
+    <t>Assume price product =</t>
+  </si>
+  <si>
+    <t>USD / customer</t>
+  </si>
+  <si>
+    <t>NET REVENUE RETENTION</t>
+  </si>
+  <si>
+    <t>CUMULATIVE NET REVENUE</t>
+  </si>
+  <si>
+    <t>CUSTOMER LIFETIME VALUE</t>
   </si>
 </sst>
 </file>
@@ -441,7 +514,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +532,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -574,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -621,13 +700,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -664,6 +736,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2312,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E543FBAA-03B2-4214-9EAC-B6E525735C1D}">
   <dimension ref="A14:F101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2532,13 +2629,13 @@
       <c r="B37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="21">
+      <c r="C37" s="18">
         <f>C34+D34+E34+F34</f>
         <v>6171.4973860156315</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -2616,15 +2713,15 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="24"/>
-      <c r="C60" s="23" t="s">
+      <c r="B60" s="21"/>
+      <c r="C60" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
     </row>
     <row r="61" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B61" s="25"/>
+      <c r="B61" s="22"/>
       <c r="C61" s="9" t="s">
         <v>44</v>
       </c>
@@ -2852,13 +2949,13 @@
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B82" s="26" t="s">
+      <c r="B82" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="28"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="25"/>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" s="8" t="s">
@@ -2974,13 +3071,13 @@
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B89" s="29" t="s">
+      <c r="B89" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
-      <c r="E89" s="30"/>
-      <c r="F89" s="31"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="28"/>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90" s="9" t="s">
@@ -3059,13 +3156,13 @@
       </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B94" s="32" t="s">
+      <c r="B94" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C94" s="32"/>
-      <c r="D94" s="32"/>
-      <c r="E94" s="32"/>
-      <c r="F94" s="32"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" s="9" t="s">
@@ -3140,13 +3237,13 @@
       <c r="B100" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C100" s="21">
+      <c r="C100" s="18">
         <f>C97+D97+E97+F97</f>
         <v>649.53086419753095</v>
       </c>
-      <c r="D100" s="22"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="22"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="19"/>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="1"/>
@@ -3170,7 +3267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34660E54-E454-4585-B1D5-AED39921E2E1}">
   <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+    <sheetView topLeftCell="A74" workbookViewId="0">
       <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
@@ -3602,8 +3699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14953EC9-AD0E-4C14-A329-458979F57CAE}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3614,336 +3711,399 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="35"/>
+      <c r="E1" s="39" t="s">
         <v>119</v>
       </c>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E2" s="1" t="s">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="E2" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="35">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="35">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="35">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="35">
         <v>3</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="35">
         <v>4</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="35">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="37">
         <v>500</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="35">
         <v>100000</v>
       </c>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="37">
         <v>1000</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="35">
         <v>200</v>
       </c>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
     </row>
     <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="37">
         <v>0.75</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="35">
         <f>F3/F4</f>
         <v>500</v>
       </c>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="35"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="35">
         <f>1-B5</f>
         <v>0.25</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="G7">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35">
         <v>500</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="35">
         <v>1000</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="35">
         <v>1500</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="35">
         <v>2000</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="35">
         <v>2500</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="35">
         <f>1/B7</f>
         <v>4</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="G8">
+      <c r="F8" s="35"/>
+      <c r="G8" s="35">
         <f>G7*0.6</f>
         <v>300</v>
       </c>
-      <c r="H8">
-        <f t="shared" ref="H8:K8" si="0">H7*0.6</f>
+      <c r="H8" s="35">
+        <f>H7*0.6</f>
         <v>600</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
+      <c r="I8" s="35">
+        <f t="shared" ref="H8:K8" si="0">I7*0.6</f>
         <v>900</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="35">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="35">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E9" s="1" t="s">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="E9" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="G9">
+      <c r="F9" s="35"/>
+      <c r="G9" s="35">
         <f>G7-G8</f>
         <v>200</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="35">
         <f t="shared" ref="H9:K9" si="1">H7-H8</f>
         <v>400</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
+      <c r="I9" s="35">
+        <f>I7-I8</f>
         <v>600</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="35">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="35">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="35">
         <f>B4*B8-B3</f>
         <v>3500</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
     </row>
     <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="G11">
+      <c r="F11" s="35"/>
+      <c r="G11" s="35">
         <v>1</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="35">
         <v>0.6</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="35">
         <v>0.65</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="35">
         <v>0.7</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="35">
         <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="G12" s="2">
+      <c r="F12" s="35"/>
+      <c r="G12" s="40">
         <f>G11</f>
         <v>1</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="40">
         <f>G12*H11</f>
         <v>0.6</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="40">
         <f>H12*I11</f>
         <v>0.39</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="40">
         <f>I12*J11</f>
         <v>0.27299999999999996</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="40">
         <f>J12*K11</f>
         <v>0.20474999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="G14">
+      <c r="F14" s="35"/>
+      <c r="G14" s="35">
         <f>G12*G9</f>
         <v>200</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="35">
         <f>H12*H9</f>
         <v>240</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="35">
         <f t="shared" ref="I14:K14" si="2">I12*I9</f>
         <v>234</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="35">
         <f t="shared" si="2"/>
         <v>218.39999999999998</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="35">
         <f t="shared" si="2"/>
         <v>204.75</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E15" s="1"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="35">
         <v>1</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="35">
         <f>(1+0.1)^1</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="35">
         <f>(1+0.1)^2</f>
         <v>1.2100000000000002</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="35">
         <f>(1+0.1)^3</f>
         <v>1.3310000000000004</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="35">
         <f>(1+0.1)^4</f>
         <v>1.4641000000000004</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="35">
         <f>(1+0.1)^5</f>
         <v>1.6105100000000006</v>
       </c>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E17" s="1"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="35">
         <v>500</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="35">
         <f>G14/G16</f>
         <v>181.81818181818181</v>
       </c>
-      <c r="H18">
-        <f t="shared" ref="H18:K18" si="3">H14/H16</f>
+      <c r="H18" s="35">
+        <f>H14/H16</f>
         <v>198.34710743801651</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="3"/>
+      <c r="I18" s="35">
+        <f>I14/I16</f>
         <v>175.80766341096916</v>
       </c>
-      <c r="J18">
-        <f t="shared" si="3"/>
+      <c r="J18" s="35">
+        <f t="shared" ref="H18:K18" si="3">J14/J16</f>
         <v>149.17013865173138</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="35">
         <f t="shared" si="3"/>
         <v>127.13364089636198</v>
       </c>
     </row>
     <row r="19" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="35">
         <v>-500</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="35">
         <f>F19+G18</f>
         <v>-318.18181818181819</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="35">
         <f>G19+H18</f>
         <v>-119.83471074380168</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="35">
         <f>H19+I18</f>
         <v>55.972952667167476</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="35">
         <f>I19+J18</f>
         <v>205.14309131889885</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="35">
         <f>J19+K18</f>
         <v>332.27673221526084</v>
       </c>
@@ -3970,6 +4130,3402 @@
       <c r="E26" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F1BF13-F317-4922-A919-5B170DF3EC52}">
+  <dimension ref="A1:O97"/>
+  <sheetViews>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="15" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="30">
+        <v>0</v>
+      </c>
+      <c r="E5" s="30">
+        <v>1</v>
+      </c>
+      <c r="F5" s="30">
+        <v>2</v>
+      </c>
+      <c r="G5" s="30">
+        <v>3</v>
+      </c>
+      <c r="H5" s="30">
+        <v>4</v>
+      </c>
+      <c r="I5" s="30">
+        <v>5</v>
+      </c>
+      <c r="J5" s="30">
+        <v>6</v>
+      </c>
+      <c r="K5" s="30">
+        <v>7</v>
+      </c>
+      <c r="L5" s="30">
+        <v>8</v>
+      </c>
+      <c r="M5" s="30">
+        <v>9</v>
+      </c>
+      <c r="N5" s="30">
+        <v>10</v>
+      </c>
+      <c r="O5" s="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="30">
+        <v>0</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="8">
+        <v>35</v>
+      </c>
+      <c r="E6" s="8">
+        <v>35</v>
+      </c>
+      <c r="F6" s="8">
+        <v>30</v>
+      </c>
+      <c r="G6" s="8">
+        <v>26</v>
+      </c>
+      <c r="H6" s="8">
+        <v>25</v>
+      </c>
+      <c r="I6" s="8">
+        <v>24</v>
+      </c>
+      <c r="J6" s="8">
+        <v>22</v>
+      </c>
+      <c r="K6" s="8">
+        <v>22</v>
+      </c>
+      <c r="L6" s="8">
+        <v>20</v>
+      </c>
+      <c r="M6" s="8">
+        <v>18</v>
+      </c>
+      <c r="N6" s="8">
+        <v>15</v>
+      </c>
+      <c r="O6" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="30">
+        <v>1</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="8">
+        <v>18</v>
+      </c>
+      <c r="E7" s="8">
+        <v>18</v>
+      </c>
+      <c r="F7" s="8">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8">
+        <v>15</v>
+      </c>
+      <c r="H7" s="8">
+        <v>13</v>
+      </c>
+      <c r="I7" s="8">
+        <v>13</v>
+      </c>
+      <c r="J7" s="8">
+        <v>12</v>
+      </c>
+      <c r="K7" s="8">
+        <v>11</v>
+      </c>
+      <c r="L7" s="8">
+        <v>10</v>
+      </c>
+      <c r="M7" s="8">
+        <v>9</v>
+      </c>
+      <c r="N7" s="8">
+        <v>9</v>
+      </c>
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="30">
+        <v>2</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="8">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8">
+        <v>22</v>
+      </c>
+      <c r="F8" s="8">
+        <v>21</v>
+      </c>
+      <c r="G8" s="8">
+        <v>19</v>
+      </c>
+      <c r="H8" s="8">
+        <v>17</v>
+      </c>
+      <c r="I8" s="8">
+        <v>17</v>
+      </c>
+      <c r="J8" s="8">
+        <v>15</v>
+      </c>
+      <c r="K8" s="8">
+        <v>11</v>
+      </c>
+      <c r="L8" s="8">
+        <v>10</v>
+      </c>
+      <c r="M8" s="8">
+        <v>9</v>
+      </c>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="30">
+        <v>3</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="8">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8">
+        <v>18</v>
+      </c>
+      <c r="H9" s="8">
+        <v>17</v>
+      </c>
+      <c r="I9" s="8">
+        <v>16</v>
+      </c>
+      <c r="J9" s="8">
+        <v>14</v>
+      </c>
+      <c r="K9" s="8">
+        <v>9</v>
+      </c>
+      <c r="L9" s="8">
+        <v>9</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="30">
+        <v>4</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="8">
+        <v>26</v>
+      </c>
+      <c r="E10" s="8">
+        <v>26</v>
+      </c>
+      <c r="F10" s="8">
+        <v>25</v>
+      </c>
+      <c r="G10" s="8">
+        <v>23</v>
+      </c>
+      <c r="H10" s="8">
+        <v>19</v>
+      </c>
+      <c r="I10" s="8">
+        <v>18</v>
+      </c>
+      <c r="J10" s="8">
+        <v>17</v>
+      </c>
+      <c r="K10" s="8">
+        <v>15</v>
+      </c>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="30">
+        <v>5</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="8">
+        <v>20</v>
+      </c>
+      <c r="E11" s="8">
+        <v>20</v>
+      </c>
+      <c r="F11" s="8">
+        <v>19</v>
+      </c>
+      <c r="G11" s="8">
+        <v>19</v>
+      </c>
+      <c r="H11" s="8">
+        <v>19</v>
+      </c>
+      <c r="I11" s="8">
+        <v>16</v>
+      </c>
+      <c r="J11" s="8">
+        <v>14</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="30">
+        <v>6</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="8">
+        <v>22</v>
+      </c>
+      <c r="E12" s="8">
+        <v>22</v>
+      </c>
+      <c r="F12" s="8">
+        <v>20</v>
+      </c>
+      <c r="G12" s="8">
+        <v>20</v>
+      </c>
+      <c r="H12" s="8">
+        <v>19</v>
+      </c>
+      <c r="I12" s="8">
+        <v>18</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="30">
+        <v>7</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="8">
+        <v>22</v>
+      </c>
+      <c r="E13" s="8">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8">
+        <v>19</v>
+      </c>
+      <c r="G13" s="8">
+        <v>17</v>
+      </c>
+      <c r="H13" s="8">
+        <v>13</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="30">
+        <v>8</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="8">
+        <v>19</v>
+      </c>
+      <c r="E14" s="8">
+        <v>19</v>
+      </c>
+      <c r="F14" s="8">
+        <v>19</v>
+      </c>
+      <c r="G14" s="8">
+        <v>17</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="30">
+        <v>9</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="8">
+        <v>23</v>
+      </c>
+      <c r="E15" s="8">
+        <v>23</v>
+      </c>
+      <c r="F15" s="8">
+        <v>23</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="30">
+        <v>10</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="8">
+        <v>12</v>
+      </c>
+      <c r="E16" s="8">
+        <v>12</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="30">
+        <v>11</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="8">
+        <v>16</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="30">
+        <v>0</v>
+      </c>
+      <c r="E21" s="30">
+        <v>1</v>
+      </c>
+      <c r="F21" s="30">
+        <v>2</v>
+      </c>
+      <c r="G21" s="30">
+        <v>3</v>
+      </c>
+      <c r="H21" s="30">
+        <v>4</v>
+      </c>
+      <c r="I21" s="30">
+        <v>5</v>
+      </c>
+      <c r="J21" s="30">
+        <v>6</v>
+      </c>
+      <c r="K21" s="30">
+        <v>7</v>
+      </c>
+      <c r="L21" s="30">
+        <v>8</v>
+      </c>
+      <c r="M21" s="30">
+        <v>9</v>
+      </c>
+      <c r="N21" s="30">
+        <v>10</v>
+      </c>
+      <c r="O21" s="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="30">
+        <v>0</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="32">
+        <f>D6/$D$6</f>
+        <v>1</v>
+      </c>
+      <c r="E22" s="32">
+        <f>E6/$D$6</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="32">
+        <f>F6/$D$6</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G22" s="32">
+        <f t="shared" ref="E22:O22" si="0">G6/$D$6</f>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="H22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="I22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.68571428571428572</v>
+      </c>
+      <c r="J22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.62857142857142856</v>
+      </c>
+      <c r="K22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.62857142857142856</v>
+      </c>
+      <c r="L22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="M22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.51428571428571423</v>
+      </c>
+      <c r="N22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="O22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.25714285714285712</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B23" s="30">
+        <v>1</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="32">
+        <f>D7/$D$7</f>
+        <v>1</v>
+      </c>
+      <c r="E23" s="32">
+        <f t="shared" ref="E23:O23" si="1">E7/$D$7</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="G23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="I23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="J23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="L23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="M23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="N23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="O23" s="32"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B24" s="30">
+        <v>2</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="32">
+        <f>D8/$D$8</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="32">
+        <f t="shared" ref="E24:M24" si="2">E8/$D$8</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="32">
+        <f t="shared" si="2"/>
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="G24" s="32">
+        <f t="shared" si="2"/>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="H24" s="32">
+        <f t="shared" si="2"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="I24" s="32">
+        <f t="shared" si="2"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="J24" s="32">
+        <f t="shared" si="2"/>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="K24" s="32">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="L24" s="32">
+        <f t="shared" si="2"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="M24" s="32">
+        <f t="shared" si="2"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B25" s="30">
+        <v>3</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25" s="32">
+        <f>D9/$D$9</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="32">
+        <f t="shared" ref="E25:L25" si="3">E9/$D$9</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="32">
+        <f t="shared" si="3"/>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="G25" s="32">
+        <f t="shared" si="3"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="H25" s="32">
+        <f t="shared" si="3"/>
+        <v>0.80952380952380953</v>
+      </c>
+      <c r="I25" s="32">
+        <f t="shared" si="3"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="J25" s="32">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K25" s="32">
+        <f t="shared" si="3"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="L25" s="32">
+        <f t="shared" si="3"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B26" s="30">
+        <v>4</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="32">
+        <f>D10/$D$10</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="32">
+        <f t="shared" ref="E26:K26" si="4">E10/$D$10</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="32">
+        <f t="shared" si="4"/>
+        <v>0.96153846153846156</v>
+      </c>
+      <c r="G26" s="32">
+        <f t="shared" si="4"/>
+        <v>0.88461538461538458</v>
+      </c>
+      <c r="H26" s="32">
+        <f t="shared" si="4"/>
+        <v>0.73076923076923073</v>
+      </c>
+      <c r="I26" s="32">
+        <f t="shared" si="4"/>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="J26" s="32">
+        <f t="shared" si="4"/>
+        <v>0.65384615384615385</v>
+      </c>
+      <c r="K26" s="32">
+        <f t="shared" si="4"/>
+        <v>0.57692307692307687</v>
+      </c>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B27" s="30">
+        <v>5</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="32">
+        <f>D11/$D$11</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="32">
+        <f t="shared" ref="E27:J27" si="5">E11/$D$11</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="32">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="G27" s="32">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="H27" s="32">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="I27" s="32">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="J27" s="32">
+        <f t="shared" si="5"/>
+        <v>0.7</v>
+      </c>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B28" s="30">
+        <v>6</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="32">
+        <f>D12/$D$12</f>
+        <v>1</v>
+      </c>
+      <c r="E28" s="32">
+        <f t="shared" ref="E28:I28" si="6">E12/$D$12</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="32">
+        <f t="shared" si="6"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="G28" s="32">
+        <f t="shared" si="6"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="H28" s="32">
+        <f t="shared" si="6"/>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="I28" s="32">
+        <f t="shared" si="6"/>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B29" s="30">
+        <v>7</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="32">
+        <f>D13/$D$13</f>
+        <v>1</v>
+      </c>
+      <c r="E29" s="32">
+        <f t="shared" ref="E29:H29" si="7">E13/$D$13</f>
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="F29" s="32">
+        <f t="shared" si="7"/>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="G29" s="32">
+        <f t="shared" si="7"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="H29" s="32">
+        <f t="shared" si="7"/>
+        <v>0.59090909090909094</v>
+      </c>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B30" s="30">
+        <v>8</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="32">
+        <f>D14/$D$14</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="32">
+        <f t="shared" ref="E30:G30" si="8">E14/$D$14</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="32">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G30" s="32">
+        <f t="shared" si="8"/>
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B31" s="30">
+        <v>9</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="32">
+        <f>D15/$D$15</f>
+        <v>1</v>
+      </c>
+      <c r="E31" s="32">
+        <f t="shared" ref="E31:F31" si="9">E15/$D$15</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="32">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B32" s="30">
+        <v>10</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="32">
+        <f>D16/$D$16</f>
+        <v>1</v>
+      </c>
+      <c r="E32" s="32">
+        <f>E16/$D$16</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B33" s="30">
+        <v>11</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="32">
+        <f>D17/$D$17</f>
+        <v>1</v>
+      </c>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35">
+        <v>50</v>
+      </c>
+      <c r="F35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B36" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B37" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="30">
+        <v>0</v>
+      </c>
+      <c r="E37" s="30">
+        <v>1</v>
+      </c>
+      <c r="F37" s="30">
+        <v>2</v>
+      </c>
+      <c r="G37" s="30">
+        <v>3</v>
+      </c>
+      <c r="H37" s="30">
+        <v>4</v>
+      </c>
+      <c r="I37" s="30">
+        <v>5</v>
+      </c>
+      <c r="J37" s="30">
+        <v>6</v>
+      </c>
+      <c r="K37" s="30">
+        <v>7</v>
+      </c>
+      <c r="L37" s="30">
+        <v>8</v>
+      </c>
+      <c r="M37" s="30">
+        <v>9</v>
+      </c>
+      <c r="N37" s="30">
+        <v>10</v>
+      </c>
+      <c r="O37" s="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B38" s="30">
+        <v>0</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="8">
+        <f>$E$35*D6</f>
+        <v>1750</v>
+      </c>
+      <c r="E38" s="8">
+        <f>$E$35*E6</f>
+        <v>1750</v>
+      </c>
+      <c r="F38" s="8">
+        <f t="shared" ref="E38:O38" si="10">$E$35*F6</f>
+        <v>1500</v>
+      </c>
+      <c r="G38" s="8">
+        <f t="shared" si="10"/>
+        <v>1300</v>
+      </c>
+      <c r="H38" s="8">
+        <f t="shared" si="10"/>
+        <v>1250</v>
+      </c>
+      <c r="I38" s="8">
+        <f t="shared" si="10"/>
+        <v>1200</v>
+      </c>
+      <c r="J38" s="8">
+        <f t="shared" si="10"/>
+        <v>1100</v>
+      </c>
+      <c r="K38" s="8">
+        <f t="shared" si="10"/>
+        <v>1100</v>
+      </c>
+      <c r="L38" s="8">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="M38" s="8">
+        <f t="shared" si="10"/>
+        <v>900</v>
+      </c>
+      <c r="N38" s="8">
+        <f t="shared" si="10"/>
+        <v>750</v>
+      </c>
+      <c r="O38" s="8">
+        <f t="shared" si="10"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B39" s="30">
+        <v>1</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" s="8">
+        <f t="shared" ref="D39:O39" si="11">$E$35*D7</f>
+        <v>900</v>
+      </c>
+      <c r="E39" s="8">
+        <f t="shared" si="11"/>
+        <v>900</v>
+      </c>
+      <c r="F39" s="8">
+        <f t="shared" si="11"/>
+        <v>800</v>
+      </c>
+      <c r="G39" s="8">
+        <f t="shared" si="11"/>
+        <v>750</v>
+      </c>
+      <c r="H39" s="8">
+        <f t="shared" si="11"/>
+        <v>650</v>
+      </c>
+      <c r="I39" s="8">
+        <f t="shared" si="11"/>
+        <v>650</v>
+      </c>
+      <c r="J39" s="8">
+        <f t="shared" si="11"/>
+        <v>600</v>
+      </c>
+      <c r="K39" s="8">
+        <f t="shared" si="11"/>
+        <v>550</v>
+      </c>
+      <c r="L39" s="8">
+        <f t="shared" si="11"/>
+        <v>500</v>
+      </c>
+      <c r="M39" s="8">
+        <f t="shared" si="11"/>
+        <v>450</v>
+      </c>
+      <c r="N39" s="8">
+        <f t="shared" si="11"/>
+        <v>450</v>
+      </c>
+      <c r="O39" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B40" s="30">
+        <v>2</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D40" s="8">
+        <f t="shared" ref="D40:O40" si="12">$E$35*D8</f>
+        <v>1100</v>
+      </c>
+      <c r="E40" s="8">
+        <f t="shared" si="12"/>
+        <v>1100</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="12"/>
+        <v>1050</v>
+      </c>
+      <c r="G40" s="8">
+        <f t="shared" si="12"/>
+        <v>950</v>
+      </c>
+      <c r="H40" s="8">
+        <f t="shared" si="12"/>
+        <v>850</v>
+      </c>
+      <c r="I40" s="8">
+        <f t="shared" si="12"/>
+        <v>850</v>
+      </c>
+      <c r="J40" s="8">
+        <f t="shared" si="12"/>
+        <v>750</v>
+      </c>
+      <c r="K40" s="8">
+        <f t="shared" si="12"/>
+        <v>550</v>
+      </c>
+      <c r="L40" s="8">
+        <f t="shared" si="12"/>
+        <v>500</v>
+      </c>
+      <c r="M40" s="8">
+        <f t="shared" si="12"/>
+        <v>450</v>
+      </c>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B41" s="30">
+        <v>3</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" s="8">
+        <f t="shared" ref="D41:O41" si="13">$E$35*D9</f>
+        <v>1050</v>
+      </c>
+      <c r="E41" s="8">
+        <f t="shared" si="13"/>
+        <v>1050</v>
+      </c>
+      <c r="F41" s="8">
+        <f t="shared" si="13"/>
+        <v>1000</v>
+      </c>
+      <c r="G41" s="8">
+        <f t="shared" si="13"/>
+        <v>900</v>
+      </c>
+      <c r="H41" s="8">
+        <f t="shared" si="13"/>
+        <v>850</v>
+      </c>
+      <c r="I41" s="8">
+        <f t="shared" si="13"/>
+        <v>800</v>
+      </c>
+      <c r="J41" s="8">
+        <f t="shared" si="13"/>
+        <v>700</v>
+      </c>
+      <c r="K41" s="8">
+        <f t="shared" si="13"/>
+        <v>450</v>
+      </c>
+      <c r="L41" s="8">
+        <f t="shared" si="13"/>
+        <v>450</v>
+      </c>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B42" s="30">
+        <v>4</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="8">
+        <f t="shared" ref="D42:O42" si="14">$E$35*D10</f>
+        <v>1300</v>
+      </c>
+      <c r="E42" s="8">
+        <f t="shared" si="14"/>
+        <v>1300</v>
+      </c>
+      <c r="F42" s="8">
+        <f t="shared" si="14"/>
+        <v>1250</v>
+      </c>
+      <c r="G42" s="8">
+        <f t="shared" si="14"/>
+        <v>1150</v>
+      </c>
+      <c r="H42" s="8">
+        <f t="shared" si="14"/>
+        <v>950</v>
+      </c>
+      <c r="I42" s="8">
+        <f t="shared" si="14"/>
+        <v>900</v>
+      </c>
+      <c r="J42" s="8">
+        <f t="shared" si="14"/>
+        <v>850</v>
+      </c>
+      <c r="K42" s="8">
+        <f t="shared" si="14"/>
+        <v>750</v>
+      </c>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B43" s="30">
+        <v>5</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="8">
+        <f t="shared" ref="D43:O43" si="15">$E$35*D11</f>
+        <v>1000</v>
+      </c>
+      <c r="E43" s="8">
+        <f t="shared" si="15"/>
+        <v>1000</v>
+      </c>
+      <c r="F43" s="8">
+        <f t="shared" si="15"/>
+        <v>950</v>
+      </c>
+      <c r="G43" s="8">
+        <f t="shared" si="15"/>
+        <v>950</v>
+      </c>
+      <c r="H43" s="8">
+        <f t="shared" si="15"/>
+        <v>950</v>
+      </c>
+      <c r="I43" s="8">
+        <f t="shared" si="15"/>
+        <v>800</v>
+      </c>
+      <c r="J43" s="8">
+        <f t="shared" si="15"/>
+        <v>700</v>
+      </c>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B44" s="30">
+        <v>6</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" s="8">
+        <f t="shared" ref="D44:O44" si="16">$E$35*D12</f>
+        <v>1100</v>
+      </c>
+      <c r="E44" s="8">
+        <f t="shared" si="16"/>
+        <v>1100</v>
+      </c>
+      <c r="F44" s="8">
+        <f t="shared" si="16"/>
+        <v>1000</v>
+      </c>
+      <c r="G44" s="8">
+        <f t="shared" si="16"/>
+        <v>1000</v>
+      </c>
+      <c r="H44" s="8">
+        <f t="shared" si="16"/>
+        <v>950</v>
+      </c>
+      <c r="I44" s="8">
+        <f t="shared" si="16"/>
+        <v>900</v>
+      </c>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B45" s="30">
+        <v>7</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" s="8">
+        <f t="shared" ref="D45:O45" si="17">$E$35*D13</f>
+        <v>1100</v>
+      </c>
+      <c r="E45" s="8">
+        <f t="shared" si="17"/>
+        <v>1050</v>
+      </c>
+      <c r="F45" s="8">
+        <f t="shared" si="17"/>
+        <v>950</v>
+      </c>
+      <c r="G45" s="8">
+        <f t="shared" si="17"/>
+        <v>850</v>
+      </c>
+      <c r="H45" s="8">
+        <f t="shared" si="17"/>
+        <v>650</v>
+      </c>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B46" s="30">
+        <v>8</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D46" s="8">
+        <f t="shared" ref="D46:O46" si="18">$E$35*D14</f>
+        <v>950</v>
+      </c>
+      <c r="E46" s="8">
+        <f t="shared" si="18"/>
+        <v>950</v>
+      </c>
+      <c r="F46" s="8">
+        <f t="shared" si="18"/>
+        <v>950</v>
+      </c>
+      <c r="G46" s="8">
+        <f t="shared" si="18"/>
+        <v>850</v>
+      </c>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B47" s="30">
+        <v>9</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" s="8">
+        <f t="shared" ref="D47:O47" si="19">$E$35*D15</f>
+        <v>1150</v>
+      </c>
+      <c r="E47" s="8">
+        <f t="shared" si="19"/>
+        <v>1150</v>
+      </c>
+      <c r="F47" s="8">
+        <f t="shared" si="19"/>
+        <v>1150</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B48" s="30">
+        <v>10</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" s="8">
+        <f t="shared" ref="D48:O48" si="20">$E$35*D16</f>
+        <v>600</v>
+      </c>
+      <c r="E48" s="8">
+        <f t="shared" si="20"/>
+        <v>600</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B49" s="30">
+        <v>11</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D49" s="8">
+        <f t="shared" ref="D49:O49" si="21">$E$35*D17</f>
+        <v>800</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B52" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B53" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="30">
+        <v>0</v>
+      </c>
+      <c r="E53" s="30">
+        <v>1</v>
+      </c>
+      <c r="F53" s="30">
+        <v>2</v>
+      </c>
+      <c r="G53" s="30">
+        <v>3</v>
+      </c>
+      <c r="H53" s="30">
+        <v>4</v>
+      </c>
+      <c r="I53" s="30">
+        <v>5</v>
+      </c>
+      <c r="J53" s="30">
+        <v>6</v>
+      </c>
+      <c r="K53" s="30">
+        <v>7</v>
+      </c>
+      <c r="L53" s="30">
+        <v>8</v>
+      </c>
+      <c r="M53" s="30">
+        <v>9</v>
+      </c>
+      <c r="N53" s="30">
+        <v>10</v>
+      </c>
+      <c r="O53" s="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B54" s="30">
+        <v>0</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" s="32">
+        <f>D38/$D$38</f>
+        <v>1</v>
+      </c>
+      <c r="E54" s="32">
+        <f t="shared" ref="E54:O54" si="22">E38/$D$38</f>
+        <v>1</v>
+      </c>
+      <c r="F54" s="32">
+        <f>F38/$D$38</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G54" s="32">
+        <f t="shared" si="22"/>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="H54" s="32">
+        <f t="shared" si="22"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="I54" s="32">
+        <f t="shared" si="22"/>
+        <v>0.68571428571428572</v>
+      </c>
+      <c r="J54" s="32">
+        <f t="shared" si="22"/>
+        <v>0.62857142857142856</v>
+      </c>
+      <c r="K54" s="32">
+        <f t="shared" si="22"/>
+        <v>0.62857142857142856</v>
+      </c>
+      <c r="L54" s="32">
+        <f t="shared" si="22"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="M54" s="32">
+        <f t="shared" si="22"/>
+        <v>0.51428571428571423</v>
+      </c>
+      <c r="N54" s="32">
+        <f t="shared" si="22"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="O54" s="32">
+        <f t="shared" si="22"/>
+        <v>0.25714285714285712</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B55" s="30">
+        <v>1</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D55" s="32">
+        <f>D39/$D$39</f>
+        <v>1</v>
+      </c>
+      <c r="E55" s="32">
+        <f t="shared" ref="E55:N55" si="23">E39/$D$39</f>
+        <v>1</v>
+      </c>
+      <c r="F55" s="32">
+        <f t="shared" si="23"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="G55" s="32">
+        <f t="shared" si="23"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H55" s="32">
+        <f t="shared" si="23"/>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="I55" s="32">
+        <f t="shared" si="23"/>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="J55" s="32">
+        <f t="shared" si="23"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K55" s="32">
+        <f t="shared" si="23"/>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="L55" s="32">
+        <f t="shared" si="23"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="M55" s="32">
+        <f t="shared" si="23"/>
+        <v>0.5</v>
+      </c>
+      <c r="N55" s="32">
+        <f t="shared" si="23"/>
+        <v>0.5</v>
+      </c>
+      <c r="O55" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B56" s="30">
+        <v>2</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D56" s="32">
+        <f>D40/$D$40</f>
+        <v>1</v>
+      </c>
+      <c r="E56" s="32">
+        <f t="shared" ref="E56:M56" si="24">E40/$D$40</f>
+        <v>1</v>
+      </c>
+      <c r="F56" s="32">
+        <f t="shared" si="24"/>
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="G56" s="32">
+        <f t="shared" si="24"/>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="H56" s="32">
+        <f t="shared" si="24"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="I56" s="32">
+        <f t="shared" si="24"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="J56" s="32">
+        <f t="shared" si="24"/>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="K56" s="32">
+        <f t="shared" si="24"/>
+        <v>0.5</v>
+      </c>
+      <c r="L56" s="32">
+        <f t="shared" si="24"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="M56" s="32">
+        <f t="shared" si="24"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="N56" s="32"/>
+      <c r="O56" s="32"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B57" s="30">
+        <v>3</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" s="32">
+        <f>D41/$D$41</f>
+        <v>1</v>
+      </c>
+      <c r="E57" s="32">
+        <f t="shared" ref="E57:L57" si="25">E41/$D$41</f>
+        <v>1</v>
+      </c>
+      <c r="F57" s="32">
+        <f t="shared" si="25"/>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="G57" s="32">
+        <f t="shared" si="25"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="H57" s="32">
+        <f t="shared" si="25"/>
+        <v>0.80952380952380953</v>
+      </c>
+      <c r="I57" s="32">
+        <f t="shared" si="25"/>
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="J57" s="32">
+        <f t="shared" si="25"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K57" s="32">
+        <f t="shared" si="25"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="L57" s="32">
+        <f t="shared" si="25"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="M57" s="32"/>
+      <c r="N57" s="32"/>
+      <c r="O57" s="32"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B58" s="30">
+        <v>4</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D58" s="32">
+        <f>D42/$D$42</f>
+        <v>1</v>
+      </c>
+      <c r="E58" s="32">
+        <f t="shared" ref="E58:K58" si="26">E42/$D$42</f>
+        <v>1</v>
+      </c>
+      <c r="F58" s="32">
+        <f t="shared" si="26"/>
+        <v>0.96153846153846156</v>
+      </c>
+      <c r="G58" s="32">
+        <f t="shared" si="26"/>
+        <v>0.88461538461538458</v>
+      </c>
+      <c r="H58" s="32">
+        <f t="shared" si="26"/>
+        <v>0.73076923076923073</v>
+      </c>
+      <c r="I58" s="32">
+        <f t="shared" si="26"/>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="J58" s="32">
+        <f t="shared" si="26"/>
+        <v>0.65384615384615385</v>
+      </c>
+      <c r="K58" s="32">
+        <f t="shared" si="26"/>
+        <v>0.57692307692307687</v>
+      </c>
+      <c r="L58" s="32"/>
+      <c r="M58" s="32"/>
+      <c r="N58" s="32"/>
+      <c r="O58" s="32"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B59" s="30">
+        <v>5</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="32">
+        <f>D43/$D$43</f>
+        <v>1</v>
+      </c>
+      <c r="E59" s="32">
+        <f t="shared" ref="E59:J59" si="27">E43/$D$43</f>
+        <v>1</v>
+      </c>
+      <c r="F59" s="32">
+        <f t="shared" si="27"/>
+        <v>0.95</v>
+      </c>
+      <c r="G59" s="32">
+        <f t="shared" si="27"/>
+        <v>0.95</v>
+      </c>
+      <c r="H59" s="32">
+        <f t="shared" si="27"/>
+        <v>0.95</v>
+      </c>
+      <c r="I59" s="32">
+        <f t="shared" si="27"/>
+        <v>0.8</v>
+      </c>
+      <c r="J59" s="32">
+        <f t="shared" si="27"/>
+        <v>0.7</v>
+      </c>
+      <c r="K59" s="32"/>
+      <c r="L59" s="32"/>
+      <c r="M59" s="32"/>
+      <c r="N59" s="32"/>
+      <c r="O59" s="32"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B60" s="30">
+        <v>6</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D60" s="32">
+        <f>D44/$D$44</f>
+        <v>1</v>
+      </c>
+      <c r="E60" s="32">
+        <f t="shared" ref="E60:I60" si="28">E44/$D$44</f>
+        <v>1</v>
+      </c>
+      <c r="F60" s="32">
+        <f t="shared" si="28"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="G60" s="32">
+        <f t="shared" si="28"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="H60" s="32">
+        <f t="shared" si="28"/>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="I60" s="32">
+        <f t="shared" si="28"/>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="J60" s="32"/>
+      <c r="K60" s="32"/>
+      <c r="L60" s="32"/>
+      <c r="M60" s="32"/>
+      <c r="N60" s="32"/>
+      <c r="O60" s="32"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B61" s="30">
+        <v>7</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D61" s="32">
+        <f>D45/$D$45</f>
+        <v>1</v>
+      </c>
+      <c r="E61" s="32">
+        <f t="shared" ref="E61:H61" si="29">E45/$D$45</f>
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="F61" s="32">
+        <f t="shared" si="29"/>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="G61" s="32">
+        <f t="shared" si="29"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="H61" s="32">
+        <f t="shared" si="29"/>
+        <v>0.59090909090909094</v>
+      </c>
+      <c r="I61" s="32"/>
+      <c r="J61" s="32"/>
+      <c r="K61" s="32"/>
+      <c r="L61" s="32"/>
+      <c r="M61" s="32"/>
+      <c r="N61" s="32"/>
+      <c r="O61" s="32"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B62" s="30">
+        <v>8</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" s="32">
+        <f>D46/$D$46</f>
+        <v>1</v>
+      </c>
+      <c r="E62" s="32">
+        <f t="shared" ref="E62:G62" si="30">E46/$D$46</f>
+        <v>1</v>
+      </c>
+      <c r="F62" s="32">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="G62" s="32">
+        <f t="shared" si="30"/>
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="H62" s="32"/>
+      <c r="I62" s="32"/>
+      <c r="J62" s="32"/>
+      <c r="K62" s="32"/>
+      <c r="L62" s="32"/>
+      <c r="M62" s="32"/>
+      <c r="N62" s="32"/>
+      <c r="O62" s="32"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B63" s="30">
+        <v>9</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63" s="32">
+        <f>D47/$D$47</f>
+        <v>1</v>
+      </c>
+      <c r="E63" s="32">
+        <f t="shared" ref="E63:F63" si="31">E47/$D$47</f>
+        <v>1</v>
+      </c>
+      <c r="F63" s="32">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="32"/>
+      <c r="L63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="32"/>
+      <c r="O63" s="32"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B64" s="30">
+        <v>10</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" s="32">
+        <f>D48/$D$48</f>
+        <v>1</v>
+      </c>
+      <c r="E64" s="32">
+        <f>E48/$D$48</f>
+        <v>1</v>
+      </c>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="32"/>
+      <c r="L64" s="32"/>
+      <c r="M64" s="32"/>
+      <c r="N64" s="32"/>
+      <c r="O64" s="32"/>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B65" s="30">
+        <v>11</v>
+      </c>
+      <c r="C65" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D65" s="32">
+        <f>D49/$D$49</f>
+        <v>1</v>
+      </c>
+      <c r="E65" s="32"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="32"/>
+      <c r="L65" s="32"/>
+      <c r="M65" s="32"/>
+      <c r="N65" s="32"/>
+      <c r="O65" s="32"/>
+    </row>
+    <row r="68" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B68" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="20"/>
+      <c r="M68" s="20"/>
+      <c r="N68" s="20"/>
+      <c r="O68" s="20"/>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B69" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D69" s="30">
+        <v>0</v>
+      </c>
+      <c r="E69" s="30">
+        <v>1</v>
+      </c>
+      <c r="F69" s="30">
+        <v>2</v>
+      </c>
+      <c r="G69" s="30">
+        <v>3</v>
+      </c>
+      <c r="H69" s="30">
+        <v>4</v>
+      </c>
+      <c r="I69" s="30">
+        <v>5</v>
+      </c>
+      <c r="J69" s="30">
+        <v>6</v>
+      </c>
+      <c r="K69" s="30">
+        <v>7</v>
+      </c>
+      <c r="L69" s="30">
+        <v>8</v>
+      </c>
+      <c r="M69" s="30">
+        <v>9</v>
+      </c>
+      <c r="N69" s="30">
+        <v>10</v>
+      </c>
+      <c r="O69" s="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B70" s="30">
+        <v>0</v>
+      </c>
+      <c r="C70" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="33">
+        <f>D38</f>
+        <v>1750</v>
+      </c>
+      <c r="E70" s="33">
+        <f>D70+E38</f>
+        <v>3500</v>
+      </c>
+      <c r="F70" s="33">
+        <f t="shared" ref="F70:O70" si="32">E70+F38</f>
+        <v>5000</v>
+      </c>
+      <c r="G70" s="33">
+        <f t="shared" si="32"/>
+        <v>6300</v>
+      </c>
+      <c r="H70" s="33">
+        <f t="shared" si="32"/>
+        <v>7550</v>
+      </c>
+      <c r="I70" s="33">
+        <f t="shared" si="32"/>
+        <v>8750</v>
+      </c>
+      <c r="J70" s="33">
+        <f t="shared" si="32"/>
+        <v>9850</v>
+      </c>
+      <c r="K70" s="33">
+        <f t="shared" si="32"/>
+        <v>10950</v>
+      </c>
+      <c r="L70" s="33">
+        <f t="shared" si="32"/>
+        <v>11950</v>
+      </c>
+      <c r="M70" s="33">
+        <f t="shared" si="32"/>
+        <v>12850</v>
+      </c>
+      <c r="N70" s="33">
+        <f t="shared" si="32"/>
+        <v>13600</v>
+      </c>
+      <c r="O70" s="33">
+        <f t="shared" si="32"/>
+        <v>14050</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B71" s="30">
+        <v>1</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="33">
+        <f t="shared" ref="D71:D81" si="33">D39</f>
+        <v>900</v>
+      </c>
+      <c r="E71" s="33">
+        <f t="shared" ref="E71:O71" si="34">D71+E39</f>
+        <v>1800</v>
+      </c>
+      <c r="F71" s="33">
+        <f t="shared" si="34"/>
+        <v>2600</v>
+      </c>
+      <c r="G71" s="33">
+        <f t="shared" si="34"/>
+        <v>3350</v>
+      </c>
+      <c r="H71" s="33">
+        <f t="shared" si="34"/>
+        <v>4000</v>
+      </c>
+      <c r="I71" s="33">
+        <f t="shared" si="34"/>
+        <v>4650</v>
+      </c>
+      <c r="J71" s="33">
+        <f t="shared" si="34"/>
+        <v>5250</v>
+      </c>
+      <c r="K71" s="33">
+        <f t="shared" si="34"/>
+        <v>5800</v>
+      </c>
+      <c r="L71" s="33">
+        <f t="shared" si="34"/>
+        <v>6300</v>
+      </c>
+      <c r="M71" s="33">
+        <f t="shared" si="34"/>
+        <v>6750</v>
+      </c>
+      <c r="N71" s="33">
+        <f t="shared" si="34"/>
+        <v>7200</v>
+      </c>
+      <c r="O71" s="33"/>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B72" s="30">
+        <v>2</v>
+      </c>
+      <c r="C72" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D72" s="33">
+        <f t="shared" si="33"/>
+        <v>1100</v>
+      </c>
+      <c r="E72" s="33">
+        <f t="shared" ref="E72:O72" si="35">D72+E40</f>
+        <v>2200</v>
+      </c>
+      <c r="F72" s="33">
+        <f t="shared" si="35"/>
+        <v>3250</v>
+      </c>
+      <c r="G72" s="33">
+        <f t="shared" si="35"/>
+        <v>4200</v>
+      </c>
+      <c r="H72" s="33">
+        <f t="shared" si="35"/>
+        <v>5050</v>
+      </c>
+      <c r="I72" s="33">
+        <f t="shared" si="35"/>
+        <v>5900</v>
+      </c>
+      <c r="J72" s="33">
+        <f t="shared" si="35"/>
+        <v>6650</v>
+      </c>
+      <c r="K72" s="33">
+        <f t="shared" si="35"/>
+        <v>7200</v>
+      </c>
+      <c r="L72" s="33">
+        <f t="shared" si="35"/>
+        <v>7700</v>
+      </c>
+      <c r="M72" s="33">
+        <f t="shared" si="35"/>
+        <v>8150</v>
+      </c>
+      <c r="N72" s="33"/>
+      <c r="O72" s="33"/>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B73" s="30">
+        <v>3</v>
+      </c>
+      <c r="C73" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" s="33">
+        <f t="shared" si="33"/>
+        <v>1050</v>
+      </c>
+      <c r="E73" s="33">
+        <f t="shared" ref="E73:O73" si="36">D73+E41</f>
+        <v>2100</v>
+      </c>
+      <c r="F73" s="33">
+        <f t="shared" si="36"/>
+        <v>3100</v>
+      </c>
+      <c r="G73" s="33">
+        <f t="shared" si="36"/>
+        <v>4000</v>
+      </c>
+      <c r="H73" s="33">
+        <f t="shared" si="36"/>
+        <v>4850</v>
+      </c>
+      <c r="I73" s="33">
+        <f t="shared" si="36"/>
+        <v>5650</v>
+      </c>
+      <c r="J73" s="33">
+        <f t="shared" si="36"/>
+        <v>6350</v>
+      </c>
+      <c r="K73" s="33">
+        <f t="shared" si="36"/>
+        <v>6800</v>
+      </c>
+      <c r="L73" s="33">
+        <f t="shared" si="36"/>
+        <v>7250</v>
+      </c>
+      <c r="M73" s="33"/>
+      <c r="N73" s="33"/>
+      <c r="O73" s="33"/>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B74" s="30">
+        <v>4</v>
+      </c>
+      <c r="C74" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" s="33">
+        <f t="shared" si="33"/>
+        <v>1300</v>
+      </c>
+      <c r="E74" s="33">
+        <f t="shared" ref="E74:O74" si="37">D74+E42</f>
+        <v>2600</v>
+      </c>
+      <c r="F74" s="33">
+        <f t="shared" si="37"/>
+        <v>3850</v>
+      </c>
+      <c r="G74" s="33">
+        <f t="shared" si="37"/>
+        <v>5000</v>
+      </c>
+      <c r="H74" s="33">
+        <f t="shared" si="37"/>
+        <v>5950</v>
+      </c>
+      <c r="I74" s="33">
+        <f t="shared" si="37"/>
+        <v>6850</v>
+      </c>
+      <c r="J74" s="33">
+        <f t="shared" si="37"/>
+        <v>7700</v>
+      </c>
+      <c r="K74" s="33">
+        <f t="shared" si="37"/>
+        <v>8450</v>
+      </c>
+      <c r="L74" s="33"/>
+      <c r="M74" s="33"/>
+      <c r="N74" s="33"/>
+      <c r="O74" s="33"/>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B75" s="30">
+        <v>5</v>
+      </c>
+      <c r="C75" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D75" s="33">
+        <f t="shared" si="33"/>
+        <v>1000</v>
+      </c>
+      <c r="E75" s="33">
+        <f t="shared" ref="E75:O75" si="38">D75+E43</f>
+        <v>2000</v>
+      </c>
+      <c r="F75" s="33">
+        <f t="shared" si="38"/>
+        <v>2950</v>
+      </c>
+      <c r="G75" s="33">
+        <f t="shared" si="38"/>
+        <v>3900</v>
+      </c>
+      <c r="H75" s="33">
+        <f t="shared" si="38"/>
+        <v>4850</v>
+      </c>
+      <c r="I75" s="33">
+        <f t="shared" si="38"/>
+        <v>5650</v>
+      </c>
+      <c r="J75" s="33">
+        <f t="shared" si="38"/>
+        <v>6350</v>
+      </c>
+      <c r="K75" s="33"/>
+      <c r="L75" s="33"/>
+      <c r="M75" s="33"/>
+      <c r="N75" s="33"/>
+      <c r="O75" s="33"/>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B76" s="30">
+        <v>6</v>
+      </c>
+      <c r="C76" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D76" s="33">
+        <f t="shared" si="33"/>
+        <v>1100</v>
+      </c>
+      <c r="E76" s="33">
+        <f t="shared" ref="E76:O76" si="39">D76+E44</f>
+        <v>2200</v>
+      </c>
+      <c r="F76" s="33">
+        <f t="shared" si="39"/>
+        <v>3200</v>
+      </c>
+      <c r="G76" s="33">
+        <f t="shared" si="39"/>
+        <v>4200</v>
+      </c>
+      <c r="H76" s="33">
+        <f t="shared" si="39"/>
+        <v>5150</v>
+      </c>
+      <c r="I76" s="33">
+        <f t="shared" si="39"/>
+        <v>6050</v>
+      </c>
+      <c r="J76" s="33"/>
+      <c r="K76" s="33"/>
+      <c r="L76" s="33"/>
+      <c r="M76" s="33"/>
+      <c r="N76" s="33"/>
+      <c r="O76" s="33"/>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B77" s="30">
+        <v>7</v>
+      </c>
+      <c r="C77" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D77" s="33">
+        <f t="shared" si="33"/>
+        <v>1100</v>
+      </c>
+      <c r="E77" s="33">
+        <f t="shared" ref="E77:O77" si="40">D77+E45</f>
+        <v>2150</v>
+      </c>
+      <c r="F77" s="33">
+        <f t="shared" si="40"/>
+        <v>3100</v>
+      </c>
+      <c r="G77" s="33">
+        <f t="shared" si="40"/>
+        <v>3950</v>
+      </c>
+      <c r="H77" s="33">
+        <f t="shared" si="40"/>
+        <v>4600</v>
+      </c>
+      <c r="I77" s="33"/>
+      <c r="J77" s="33"/>
+      <c r="K77" s="33"/>
+      <c r="L77" s="33"/>
+      <c r="M77" s="33"/>
+      <c r="N77" s="33"/>
+      <c r="O77" s="33"/>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B78" s="30">
+        <v>8</v>
+      </c>
+      <c r="C78" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D78" s="33">
+        <f t="shared" si="33"/>
+        <v>950</v>
+      </c>
+      <c r="E78" s="33">
+        <f t="shared" ref="E78:O78" si="41">D78+E46</f>
+        <v>1900</v>
+      </c>
+      <c r="F78" s="33">
+        <f t="shared" si="41"/>
+        <v>2850</v>
+      </c>
+      <c r="G78" s="33">
+        <f t="shared" si="41"/>
+        <v>3700</v>
+      </c>
+      <c r="H78" s="33"/>
+      <c r="I78" s="33"/>
+      <c r="J78" s="33"/>
+      <c r="K78" s="33"/>
+      <c r="L78" s="33"/>
+      <c r="M78" s="33"/>
+      <c r="N78" s="33"/>
+      <c r="O78" s="33"/>
+    </row>
+    <row r="79" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B79" s="30">
+        <v>9</v>
+      </c>
+      <c r="C79" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D79" s="33">
+        <f t="shared" si="33"/>
+        <v>1150</v>
+      </c>
+      <c r="E79" s="33">
+        <f t="shared" ref="E79:O79" si="42">D79+E47</f>
+        <v>2300</v>
+      </c>
+      <c r="F79" s="33">
+        <f t="shared" si="42"/>
+        <v>3450</v>
+      </c>
+      <c r="G79" s="33"/>
+      <c r="H79" s="33"/>
+      <c r="I79" s="33"/>
+      <c r="J79" s="33"/>
+      <c r="K79" s="33"/>
+      <c r="L79" s="33"/>
+      <c r="M79" s="33"/>
+      <c r="N79" s="33"/>
+      <c r="O79" s="33"/>
+    </row>
+    <row r="80" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B80" s="30">
+        <v>10</v>
+      </c>
+      <c r="C80" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D80" s="33">
+        <f t="shared" si="33"/>
+        <v>600</v>
+      </c>
+      <c r="E80" s="33">
+        <f t="shared" ref="E80:O80" si="43">D80+E48</f>
+        <v>1200</v>
+      </c>
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="33"/>
+      <c r="I80" s="33"/>
+      <c r="J80" s="33"/>
+      <c r="K80" s="33"/>
+      <c r="L80" s="33"/>
+      <c r="M80" s="33"/>
+      <c r="N80" s="33"/>
+      <c r="O80" s="33"/>
+    </row>
+    <row r="81" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B81" s="30">
+        <v>11</v>
+      </c>
+      <c r="C81" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D81" s="33">
+        <f t="shared" si="33"/>
+        <v>800</v>
+      </c>
+      <c r="E81" s="33"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="33"/>
+      <c r="H81" s="33"/>
+      <c r="I81" s="33"/>
+      <c r="J81" s="33"/>
+      <c r="K81" s="33"/>
+      <c r="L81" s="33"/>
+      <c r="M81" s="33"/>
+      <c r="N81" s="33"/>
+      <c r="O81" s="33"/>
+    </row>
+    <row r="84" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B84" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="20"/>
+      <c r="J84" s="20"/>
+      <c r="K84" s="20"/>
+      <c r="L84" s="20"/>
+      <c r="M84" s="20"/>
+      <c r="N84" s="20"/>
+      <c r="O84" s="20"/>
+    </row>
+    <row r="85" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B85" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C85" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D85" s="30">
+        <v>0</v>
+      </c>
+      <c r="E85" s="30">
+        <v>1</v>
+      </c>
+      <c r="F85" s="30">
+        <v>2</v>
+      </c>
+      <c r="G85" s="30">
+        <v>3</v>
+      </c>
+      <c r="H85" s="30">
+        <v>4</v>
+      </c>
+      <c r="I85" s="30">
+        <v>5</v>
+      </c>
+      <c r="J85" s="30">
+        <v>6</v>
+      </c>
+      <c r="K85" s="30">
+        <v>7</v>
+      </c>
+      <c r="L85" s="30">
+        <v>8</v>
+      </c>
+      <c r="M85" s="30">
+        <v>9</v>
+      </c>
+      <c r="N85" s="30">
+        <v>10</v>
+      </c>
+      <c r="O85" s="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B86" s="30">
+        <v>0</v>
+      </c>
+      <c r="C86" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D86" s="33">
+        <f>(D38/D6)</f>
+        <v>50</v>
+      </c>
+      <c r="E86" s="33">
+        <f>(E38/E6)</f>
+        <v>50</v>
+      </c>
+      <c r="F86" s="33">
+        <f>(F38/F6)</f>
+        <v>50</v>
+      </c>
+      <c r="G86" s="33">
+        <f>(G38/G6)</f>
+        <v>50</v>
+      </c>
+      <c r="H86" s="33">
+        <f t="shared" ref="E86:O86" si="44">(H38/H6)</f>
+        <v>50</v>
+      </c>
+      <c r="I86" s="33">
+        <f t="shared" si="44"/>
+        <v>50</v>
+      </c>
+      <c r="J86" s="33">
+        <f t="shared" si="44"/>
+        <v>50</v>
+      </c>
+      <c r="K86" s="33">
+        <f t="shared" si="44"/>
+        <v>50</v>
+      </c>
+      <c r="L86" s="33">
+        <f>(L38/L6)</f>
+        <v>50</v>
+      </c>
+      <c r="M86" s="33">
+        <f t="shared" si="44"/>
+        <v>50</v>
+      </c>
+      <c r="N86" s="33">
+        <f t="shared" si="44"/>
+        <v>50</v>
+      </c>
+      <c r="O86" s="33">
+        <f t="shared" si="44"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B87" s="30">
+        <v>1</v>
+      </c>
+      <c r="C87" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D87" s="33">
+        <f t="shared" ref="D87:O97" si="45">D71/D7</f>
+        <v>50</v>
+      </c>
+      <c r="E87" s="33">
+        <f t="shared" si="45"/>
+        <v>100</v>
+      </c>
+      <c r="F87" s="33">
+        <f t="shared" si="45"/>
+        <v>162.5</v>
+      </c>
+      <c r="G87" s="33">
+        <f t="shared" si="45"/>
+        <v>223.33333333333334</v>
+      </c>
+      <c r="H87" s="33">
+        <f t="shared" si="45"/>
+        <v>307.69230769230768</v>
+      </c>
+      <c r="I87" s="33">
+        <f t="shared" si="45"/>
+        <v>357.69230769230768</v>
+      </c>
+      <c r="J87" s="33">
+        <f t="shared" si="45"/>
+        <v>437.5</v>
+      </c>
+      <c r="K87" s="33">
+        <f t="shared" si="45"/>
+        <v>527.27272727272725</v>
+      </c>
+      <c r="L87" s="33">
+        <f t="shared" si="45"/>
+        <v>630</v>
+      </c>
+      <c r="M87" s="33">
+        <f t="shared" si="45"/>
+        <v>750</v>
+      </c>
+      <c r="N87" s="33">
+        <f t="shared" si="45"/>
+        <v>800</v>
+      </c>
+      <c r="O87" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B88" s="30">
+        <v>2</v>
+      </c>
+      <c r="C88" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D88" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E88" s="33">
+        <f t="shared" si="45"/>
+        <v>100</v>
+      </c>
+      <c r="F88" s="33">
+        <f t="shared" si="45"/>
+        <v>154.76190476190476</v>
+      </c>
+      <c r="G88" s="33">
+        <f t="shared" si="45"/>
+        <v>221.05263157894737</v>
+      </c>
+      <c r="H88" s="33">
+        <f t="shared" si="45"/>
+        <v>297.05882352941177</v>
+      </c>
+      <c r="I88" s="33">
+        <f t="shared" si="45"/>
+        <v>347.05882352941177</v>
+      </c>
+      <c r="J88" s="33">
+        <f t="shared" si="45"/>
+        <v>443.33333333333331</v>
+      </c>
+      <c r="K88" s="33">
+        <f t="shared" si="45"/>
+        <v>654.5454545454545</v>
+      </c>
+      <c r="L88" s="33">
+        <f t="shared" si="45"/>
+        <v>770</v>
+      </c>
+      <c r="M88" s="33">
+        <f t="shared" si="45"/>
+        <v>905.55555555555554</v>
+      </c>
+      <c r="N88" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O88" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B89" s="30">
+        <v>3</v>
+      </c>
+      <c r="C89" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D89" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E89" s="33">
+        <f t="shared" si="45"/>
+        <v>100</v>
+      </c>
+      <c r="F89" s="33">
+        <f t="shared" si="45"/>
+        <v>155</v>
+      </c>
+      <c r="G89" s="33">
+        <f t="shared" si="45"/>
+        <v>222.22222222222223</v>
+      </c>
+      <c r="H89" s="33">
+        <f t="shared" si="45"/>
+        <v>285.29411764705884</v>
+      </c>
+      <c r="I89" s="33">
+        <f t="shared" si="45"/>
+        <v>353.125</v>
+      </c>
+      <c r="J89" s="33">
+        <f t="shared" si="45"/>
+        <v>453.57142857142856</v>
+      </c>
+      <c r="K89" s="33">
+        <f t="shared" si="45"/>
+        <v>755.55555555555554</v>
+      </c>
+      <c r="L89" s="33">
+        <f t="shared" si="45"/>
+        <v>805.55555555555554</v>
+      </c>
+      <c r="M89" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N89" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O89" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B90" s="30">
+        <v>4</v>
+      </c>
+      <c r="C90" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D90" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E90" s="33">
+        <f t="shared" si="45"/>
+        <v>100</v>
+      </c>
+      <c r="F90" s="33">
+        <f t="shared" si="45"/>
+        <v>154</v>
+      </c>
+      <c r="G90" s="33">
+        <f t="shared" si="45"/>
+        <v>217.39130434782609</v>
+      </c>
+      <c r="H90" s="33">
+        <f t="shared" si="45"/>
+        <v>313.15789473684208</v>
+      </c>
+      <c r="I90" s="33">
+        <f t="shared" si="45"/>
+        <v>380.55555555555554</v>
+      </c>
+      <c r="J90" s="33">
+        <f t="shared" si="45"/>
+        <v>452.94117647058823</v>
+      </c>
+      <c r="K90" s="33">
+        <f t="shared" si="45"/>
+        <v>563.33333333333337</v>
+      </c>
+      <c r="L90" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M90" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N90" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O90" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B91" s="30">
+        <v>5</v>
+      </c>
+      <c r="C91" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D91" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E91" s="33">
+        <f t="shared" si="45"/>
+        <v>100</v>
+      </c>
+      <c r="F91" s="33">
+        <f t="shared" si="45"/>
+        <v>155.26315789473685</v>
+      </c>
+      <c r="G91" s="33">
+        <f t="shared" si="45"/>
+        <v>205.26315789473685</v>
+      </c>
+      <c r="H91" s="33">
+        <f t="shared" si="45"/>
+        <v>255.26315789473685</v>
+      </c>
+      <c r="I91" s="33">
+        <f t="shared" si="45"/>
+        <v>353.125</v>
+      </c>
+      <c r="J91" s="33">
+        <f t="shared" si="45"/>
+        <v>453.57142857142856</v>
+      </c>
+      <c r="K91" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L91" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M91" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N91" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O91" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B92" s="30">
+        <v>6</v>
+      </c>
+      <c r="C92" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D92" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E92" s="33">
+        <f t="shared" si="45"/>
+        <v>100</v>
+      </c>
+      <c r="F92" s="33">
+        <f t="shared" si="45"/>
+        <v>160</v>
+      </c>
+      <c r="G92" s="33">
+        <f t="shared" si="45"/>
+        <v>210</v>
+      </c>
+      <c r="H92" s="33">
+        <f t="shared" si="45"/>
+        <v>271.05263157894734</v>
+      </c>
+      <c r="I92" s="33">
+        <f t="shared" si="45"/>
+        <v>336.11111111111109</v>
+      </c>
+      <c r="J92" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K92" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L92" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M92" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N92" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O92" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B93" s="30">
+        <v>7</v>
+      </c>
+      <c r="C93" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D93" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E93" s="33">
+        <f>E77/E13</f>
+        <v>102.38095238095238</v>
+      </c>
+      <c r="F93" s="33">
+        <f t="shared" si="45"/>
+        <v>163.15789473684211</v>
+      </c>
+      <c r="G93" s="33">
+        <f t="shared" si="45"/>
+        <v>232.35294117647058</v>
+      </c>
+      <c r="H93" s="33">
+        <f t="shared" si="45"/>
+        <v>353.84615384615387</v>
+      </c>
+      <c r="I93" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J93" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K93" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L93" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M93" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N93" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O93" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B94" s="30">
+        <v>8</v>
+      </c>
+      <c r="C94" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="D94" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E94" s="33">
+        <f t="shared" si="45"/>
+        <v>100</v>
+      </c>
+      <c r="F94" s="33">
+        <f t="shared" si="45"/>
+        <v>150</v>
+      </c>
+      <c r="G94" s="33">
+        <f t="shared" si="45"/>
+        <v>217.64705882352942</v>
+      </c>
+      <c r="H94" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I94" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J94" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K94" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L94" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M94" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N94" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O94" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B95" s="30">
+        <v>9</v>
+      </c>
+      <c r="C95" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D95" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E95" s="33">
+        <f t="shared" si="45"/>
+        <v>100</v>
+      </c>
+      <c r="F95" s="33">
+        <f t="shared" si="45"/>
+        <v>150</v>
+      </c>
+      <c r="G95" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H95" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I95" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J95" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K95" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L95" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M95" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N95" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O95" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="96" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B96" s="30">
+        <v>10</v>
+      </c>
+      <c r="C96" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D96" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E96" s="33">
+        <f t="shared" si="45"/>
+        <v>100</v>
+      </c>
+      <c r="F96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O96" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B97" s="30">
+        <v>11</v>
+      </c>
+      <c r="C97" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D97" s="33">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="E97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O97" s="33" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B84:O84"/>
+    <mergeCell ref="B4:O4"/>
+    <mergeCell ref="B20:O20"/>
+    <mergeCell ref="B36:O36"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="B52:O52"/>
+    <mergeCell ref="B68:O68"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>